<commit_message>
X and Y Linear Regression
</commit_message>
<xml_diff>
--- a/RegressionResults.xlsx
+++ b/RegressionResults.xlsx
@@ -351,7 +351,7 @@
         <v>0.3</v>
       </c>
       <c r="B1">
-        <v>0.2224476029670228</v>
+        <v>0.2244049146159082</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -359,7 +359,7 @@
         <v>0.3</v>
       </c>
       <c r="B2">
-        <v>0.2579138412915469</v>
+        <v>0.2966943850757304</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -367,7 +367,7 @@
         <v>0.3</v>
       </c>
       <c r="B3">
-        <v>0.2440763521756324</v>
+        <v>0.2841325605766061</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -375,7 +375,7 @@
         <v>0.3</v>
       </c>
       <c r="B4">
-        <v>0.2359331066822463</v>
+        <v>0.2461213919509468</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -383,7 +383,7 @@
         <v>0.3</v>
       </c>
       <c r="B5">
-        <v>0.2579106998445866</v>
+        <v>0.2586599311173301</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -391,7 +391,7 @@
         <v>0.3</v>
       </c>
       <c r="B6">
-        <v>0.2468042495012952</v>
+        <v>0.257391690361052</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -399,7 +399,7 @@
         <v>0.3</v>
       </c>
       <c r="B7">
-        <v>0.2442476648725815</v>
+        <v>0.3259311987765785</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -407,7 +407,7 @@
         <v>0.3</v>
       </c>
       <c r="B8">
-        <v>0.2368136516442831</v>
+        <v>0.2512733543594496</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -415,7 +415,7 @@
         <v>0.3</v>
       </c>
       <c r="B9">
-        <v>0.198678841703078</v>
+        <v>0.2549879519166294</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -423,7 +423,7 @@
         <v>0.3</v>
       </c>
       <c r="B10">
-        <v>0.2192830240522241</v>
+        <v>0.2504928486289062</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -431,7 +431,7 @@
         <v>0.3</v>
       </c>
       <c r="B11">
-        <v>0.3390870585694188</v>
+        <v>0.2723379812052493</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -439,7 +439,7 @@
         <v>0.3</v>
       </c>
       <c r="B12">
-        <v>0.3146044621427251</v>
+        <v>0.2663861495484068</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -447,7 +447,7 @@
         <v>0.3</v>
       </c>
       <c r="B13">
-        <v>0.3397134068097074</v>
+        <v>0.2786552465379439</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -455,7 +455,7 @@
         <v>0.3</v>
       </c>
       <c r="B14">
-        <v>0.3075038658471883</v>
+        <v>0.274846017359172</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -463,7 +463,7 @@
         <v>0.3</v>
       </c>
       <c r="B15">
-        <v>0.4083887671217994</v>
+        <v>0.2960167444859172</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -471,7 +471,7 @@
         <v>0.3</v>
       </c>
       <c r="B16">
-        <v>0.2785595957265059</v>
+        <v>0.2868891749835374</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -479,7 +479,7 @@
         <v>0.3</v>
       </c>
       <c r="B17">
-        <v>0.3407309855907243</v>
+        <v>0.2823203520770745</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -487,7 +487,7 @@
         <v>0.3</v>
       </c>
       <c r="B18">
-        <v>0.335418758393125</v>
+        <v>0.2860781212899837</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -495,7 +495,7 @@
         <v>0.3</v>
       </c>
       <c r="B19">
-        <v>0.3871373017202231</v>
+        <v>0.2884366226230255</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -503,7 +503,7 @@
         <v>0.3</v>
       </c>
       <c r="B20">
-        <v>0.3710933438684663</v>
+        <v>0.2753854648678993</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -511,7 +511,7 @@
         <v>0.6</v>
       </c>
       <c r="B21">
-        <v>0.8941342065434839</v>
+        <v>0.9567567476243846</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -519,7 +519,7 @@
         <v>0.6</v>
       </c>
       <c r="B22">
-        <v>0.8593774064934934</v>
+        <v>0.9369184755524351</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -527,7 +527,7 @@
         <v>0.6</v>
       </c>
       <c r="B23">
-        <v>0.8405214428299104</v>
+        <v>0.9752133735339363</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -535,7 +535,7 @@
         <v>0.6</v>
       </c>
       <c r="B24">
-        <v>0.8845597479096696</v>
+        <v>0.9476815634142541</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -543,7 +543,7 @@
         <v>0.6</v>
       </c>
       <c r="B25">
-        <v>0.8625345723247904</v>
+        <v>0.9509101927322186</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -551,7 +551,7 @@
         <v>0.6</v>
       </c>
       <c r="B26">
-        <v>0.9096154529297138</v>
+        <v>0.9797065874858975</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -559,7 +559,7 @@
         <v>0.6</v>
       </c>
       <c r="B27">
-        <v>0.936843778255394</v>
+        <v>0.9954497039790526</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -567,7 +567,7 @@
         <v>0.6</v>
       </c>
       <c r="B28">
-        <v>0.8710947820683188</v>
+        <v>0.9827678749595909</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -575,7 +575,7 @@
         <v>0.6</v>
       </c>
       <c r="B29">
-        <v>0.9117396061941463</v>
+        <v>0.9525434326041196</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -583,7 +583,7 @@
         <v>0.6</v>
       </c>
       <c r="B30">
-        <v>0.8884087405691616</v>
+        <v>0.9692783345695077</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -591,7 +591,7 @@
         <v>0.6</v>
       </c>
       <c r="B31">
-        <v>0.7150643511184995</v>
+        <v>0.7311670281391756</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -599,7 +599,7 @@
         <v>0.6</v>
       </c>
       <c r="B32">
-        <v>0.7791741050169492</v>
+        <v>0.7214513540791607</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -607,7 +607,7 @@
         <v>0.6</v>
       </c>
       <c r="B33">
-        <v>0.7846637982085412</v>
+        <v>0.7577111274251549</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -615,7 +615,7 @@
         <v>0.6</v>
       </c>
       <c r="B34">
-        <v>0.8380182988737133</v>
+        <v>0.7602944194184227</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -623,7 +623,7 @@
         <v>0.6</v>
       </c>
       <c r="B35">
-        <v>0.7881007465006959</v>
+        <v>0.7497657886383182</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -631,7 +631,7 @@
         <v>0.6</v>
       </c>
       <c r="B36">
-        <v>0.8121306256016254</v>
+        <v>0.7630017045606641</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -639,7 +639,7 @@
         <v>0.6</v>
       </c>
       <c r="B37">
-        <v>0.7855396964108792</v>
+        <v>0.7730196584628746</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -647,7 +647,7 @@
         <v>0.6</v>
       </c>
       <c r="B38">
-        <v>1.019728979686313</v>
+        <v>0.8292102833790396</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -655,7 +655,7 @@
         <v>0.6</v>
       </c>
       <c r="B39">
-        <v>0.8082695284891841</v>
+        <v>0.741655882791449</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -663,7 +663,7 @@
         <v>0.6</v>
       </c>
       <c r="B40">
-        <v>1.014732741215226</v>
+        <v>0.8277760975738393</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -671,7 +671,7 @@
         <v>0.9</v>
       </c>
       <c r="B41">
-        <v>0.9742001890784806</v>
+        <v>1.113178433379558</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -679,7 +679,7 @@
         <v>0.9</v>
       </c>
       <c r="B42">
-        <v>0.9553001409021533</v>
+        <v>1.119814876827882</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -687,7 +687,7 @@
         <v>0.9</v>
       </c>
       <c r="B43">
-        <v>0.8362569951740966</v>
+        <v>1.13244169552259</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -695,7 +695,7 @@
         <v>0.9</v>
       </c>
       <c r="B44">
-        <v>0.9419583457950793</v>
+        <v>1.124638494108494</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -703,7 +703,7 @@
         <v>0.9</v>
       </c>
       <c r="B45">
-        <v>0.9427896181782387</v>
+        <v>1.13606758556665</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -711,7 +711,7 @@
         <v>0.9</v>
       </c>
       <c r="B46">
-        <v>0.9452689096414701</v>
+        <v>1.089512586585638</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -719,7 +719,7 @@
         <v>0.9</v>
       </c>
       <c r="B47">
-        <v>0.911026960548476</v>
+        <v>1.143385092072646</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -727,7 +727,7 @@
         <v>0.9</v>
       </c>
       <c r="B48">
-        <v>0.9358845877800377</v>
+        <v>1.081033258374178</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -735,7 +735,7 @@
         <v>0.9</v>
       </c>
       <c r="B49">
-        <v>0.9426465897401073</v>
+        <v>1.087931894231743</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -743,7 +743,7 @@
         <v>0.9</v>
       </c>
       <c r="B50">
-        <v>0.9340568769536759</v>
+        <v>1.078409143499878</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -751,7 +751,7 @@
         <v>0.9</v>
       </c>
       <c r="B51">
-        <v>0.9570661842586929</v>
+        <v>0.8476493300129482</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -759,7 +759,7 @@
         <v>0.9</v>
       </c>
       <c r="B52">
-        <v>0.9588965227618758</v>
+        <v>0.8809575396146641</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -767,7 +767,7 @@
         <v>0.9</v>
       </c>
       <c r="B53">
-        <v>0.8795620469486565</v>
+        <v>0.8455715455120751</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -775,7 +775,7 @@
         <v>0.9</v>
       </c>
       <c r="B54">
-        <v>0.7560025931224956</v>
+        <v>0.7944703363004484</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -783,7 +783,7 @@
         <v>0.9</v>
       </c>
       <c r="B55">
-        <v>0.873750660384438</v>
+        <v>0.8390257662130134</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -791,7 +791,7 @@
         <v>0.9</v>
       </c>
       <c r="B56">
-        <v>0.8525633986347714</v>
+        <v>0.8628089257266272</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -799,7 +799,7 @@
         <v>0.9</v>
       </c>
       <c r="B57">
-        <v>0.8367891761534381</v>
+        <v>0.7710910676110356</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -807,7 +807,7 @@
         <v>0.9</v>
       </c>
       <c r="B58">
-        <v>0.8970346506912747</v>
+        <v>0.84213553014138</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -815,7 +815,7 @@
         <v>0.9</v>
       </c>
       <c r="B59">
-        <v>0.9036336512741556</v>
+        <v>0.8465664312561638</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -823,7 +823,7 @@
         <v>0.9</v>
       </c>
       <c r="B60">
-        <v>0.8936685025541706</v>
+        <v>0.8821682804450295</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -831,7 +831,7 @@
         <v>1.2</v>
       </c>
       <c r="B61">
-        <v>1.267670110703925</v>
+        <v>1.325214853092706</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -839,7 +839,7 @@
         <v>1.2</v>
       </c>
       <c r="B62">
-        <v>1.156965934174771</v>
+        <v>1.229746492657904</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -847,7 +847,7 @@
         <v>1.2</v>
       </c>
       <c r="B63">
-        <v>1.214807731886701</v>
+        <v>1.296492368661867</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -855,7 +855,7 @@
         <v>1.2</v>
       </c>
       <c r="B64">
-        <v>1.16124877533165</v>
+        <v>1.285224397640298</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -863,7 +863,7 @@
         <v>1.2</v>
       </c>
       <c r="B65">
-        <v>1.197596686736247</v>
+        <v>1.29569701553315</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -871,7 +871,7 @@
         <v>1.2</v>
       </c>
       <c r="B66">
-        <v>1.182202533253204</v>
+        <v>1.304457332121114</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -879,7 +879,7 @@
         <v>1.2</v>
       </c>
       <c r="B67">
-        <v>1.194834527395585</v>
+        <v>1.316381043502975</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -887,7 +887,7 @@
         <v>1.2</v>
       </c>
       <c r="B68">
-        <v>1.186204116063649</v>
+        <v>1.261809784173537</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -895,7 +895,7 @@
         <v>1.2</v>
       </c>
       <c r="B69">
-        <v>1.136613727104013</v>
+        <v>1.315708898749855</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -903,7 +903,7 @@
         <v>1.2</v>
       </c>
       <c r="B70">
-        <v>1.159026202299657</v>
+        <v>1.286543615954848</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -911,7 +911,7 @@
         <v>1.2</v>
       </c>
       <c r="B71">
-        <v>1.22843529771685</v>
+        <v>1.396385483695001</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -919,7 +919,7 @@
         <v>1.2</v>
       </c>
       <c r="B72">
-        <v>1.15990749929172</v>
+        <v>1.358687872728843</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -927,7 +927,7 @@
         <v>1.2</v>
       </c>
       <c r="B73">
-        <v>1.197049326281906</v>
+        <v>1.389910198365495</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -935,7 +935,7 @@
         <v>1.2</v>
       </c>
       <c r="B74">
-        <v>1.207083683879986</v>
+        <v>1.395722089557511</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -943,7 +943,7 @@
         <v>1.2</v>
       </c>
       <c r="B75">
-        <v>1.197545562870275</v>
+        <v>1.404384643787551</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -951,7 +951,7 @@
         <v>1.2</v>
       </c>
       <c r="B76">
-        <v>1.236623553250929</v>
+        <v>1.382893017324087</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -959,7 +959,7 @@
         <v>1.2</v>
       </c>
       <c r="B77">
-        <v>1.202549506911282</v>
+        <v>1.387109730679059</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -967,7 +967,7 @@
         <v>1.2</v>
       </c>
       <c r="B78">
-        <v>1.24478069338214</v>
+        <v>1.378225959106202</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -975,7 +975,7 @@
         <v>1.2</v>
       </c>
       <c r="B79">
-        <v>1.243333363508278</v>
+        <v>1.405054707522149</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -983,7 +983,7 @@
         <v>1.2</v>
       </c>
       <c r="B80">
-        <v>1.232704896919167</v>
+        <v>1.382692762728911</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -991,7 +991,7 @@
         <v>1.5</v>
       </c>
       <c r="B81">
-        <v>1.538635969098998</v>
+        <v>1.519949567282465</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -999,7 +999,7 @@
         <v>1.5</v>
       </c>
       <c r="B82">
-        <v>1.505909874799698</v>
+        <v>1.533925907495531</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1007,7 +1007,7 @@
         <v>1.5</v>
       </c>
       <c r="B83">
-        <v>1.519765747303431</v>
+        <v>1.514656491932222</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1015,7 +1015,7 @@
         <v>1.5</v>
       </c>
       <c r="B84">
-        <v>1.545129429376018</v>
+        <v>1.477481983750496</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1023,7 +1023,7 @@
         <v>1.5</v>
       </c>
       <c r="B85">
-        <v>1.535323057601914</v>
+        <v>1.459509504185802</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1031,7 +1031,7 @@
         <v>1.5</v>
       </c>
       <c r="B86">
-        <v>1.543175514401092</v>
+        <v>1.504534449453706</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1039,7 +1039,7 @@
         <v>1.5</v>
       </c>
       <c r="B87">
-        <v>1.536868814262149</v>
+        <v>1.475914230032065</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1047,7 +1047,7 @@
         <v>1.5</v>
       </c>
       <c r="B88">
-        <v>1.501323720831692</v>
+        <v>1.47569973841794</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1055,7 +1055,7 @@
         <v>1.5</v>
       </c>
       <c r="B89">
-        <v>1.44998079642945</v>
+        <v>1.492951699001821</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1063,7 +1063,7 @@
         <v>1.5</v>
       </c>
       <c r="B90">
-        <v>1.52934037251066</v>
+        <v>1.511722385280024</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1071,7 +1071,7 @@
         <v>1.5</v>
       </c>
       <c r="B91">
-        <v>1.494401368435668</v>
+        <v>1.458013303765713</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1079,7 +1079,7 @@
         <v>1.5</v>
       </c>
       <c r="B92">
-        <v>1.533575325900223</v>
+        <v>1.456531483572662</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1087,7 +1087,7 @@
         <v>1.5</v>
       </c>
       <c r="B93">
-        <v>1.512079209720177</v>
+        <v>1.439353102966979</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1095,7 +1095,7 @@
         <v>1.5</v>
       </c>
       <c r="B94">
-        <v>1.52264515077357</v>
+        <v>1.460197791533025</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1103,7 +1103,7 @@
         <v>1.5</v>
       </c>
       <c r="B95">
-        <v>1.530910194544269</v>
+        <v>1.435856058132061</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1111,7 +1111,7 @@
         <v>1.5</v>
       </c>
       <c r="B96">
-        <v>1.525670009304569</v>
+        <v>1.448038975866202</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1119,7 +1119,7 @@
         <v>1.5</v>
       </c>
       <c r="B97">
-        <v>1.518848577424393</v>
+        <v>1.391681384479898</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1127,7 +1127,7 @@
         <v>1.5</v>
       </c>
       <c r="B98">
-        <v>1.584273086741767</v>
+        <v>1.405487161002725</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1135,7 +1135,7 @@
         <v>1.5</v>
       </c>
       <c r="B99">
-        <v>1.528408184492655</v>
+        <v>1.408415131242398</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1143,7 +1143,7 @@
         <v>1.5</v>
       </c>
       <c r="B100">
-        <v>1.529647950612102</v>
+        <v>1.472233491256338</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1151,7 +1151,7 @@
         <v>1.8</v>
       </c>
       <c r="B101">
-        <v>1.800303519317012</v>
+        <v>1.789987751768453</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1159,7 +1159,7 @@
         <v>1.8</v>
       </c>
       <c r="B102">
-        <v>1.772342906583177</v>
+        <v>1.810071783112584</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1167,7 +1167,7 @@
         <v>1.8</v>
       </c>
       <c r="B103">
-        <v>1.782200400136283</v>
+        <v>1.786412341800955</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1175,7 +1175,7 @@
         <v>1.8</v>
       </c>
       <c r="B104">
-        <v>1.857192885881879</v>
+        <v>1.792416123068133</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1183,7 +1183,7 @@
         <v>1.8</v>
       </c>
       <c r="B105">
-        <v>1.741780919983299</v>
+        <v>1.773571900359829</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1191,7 +1191,7 @@
         <v>1.8</v>
       </c>
       <c r="B106">
-        <v>1.747041195439195</v>
+        <v>1.791232965615264</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1199,7 +1199,7 @@
         <v>1.8</v>
       </c>
       <c r="B107">
-        <v>1.796263240798375</v>
+        <v>1.794507787191275</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1207,7 +1207,7 @@
         <v>1.8</v>
       </c>
       <c r="B108">
-        <v>1.756285176741002</v>
+        <v>1.761265770277382</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1215,7 +1215,7 @@
         <v>1.8</v>
       </c>
       <c r="B109">
-        <v>1.750283729440021</v>
+        <v>1.805750551290381</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1223,7 +1223,7 @@
         <v>1.8</v>
       </c>
       <c r="B110">
-        <v>1.770417809517468</v>
+        <v>1.763610986578727</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1231,7 +1231,7 @@
         <v>1.8</v>
       </c>
       <c r="B111">
-        <v>1.800309973192597</v>
+        <v>1.745122541263489</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1239,7 +1239,7 @@
         <v>1.8</v>
       </c>
       <c r="B112">
-        <v>1.858816692291995</v>
+        <v>1.701120187425618</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1247,7 +1247,7 @@
         <v>1.8</v>
       </c>
       <c r="B113">
-        <v>1.825683850373558</v>
+        <v>1.76479639925543</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1255,7 +1255,7 @@
         <v>1.8</v>
       </c>
       <c r="B114">
-        <v>1.86287329237615</v>
+        <v>1.759680772939097</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1263,7 +1263,7 @@
         <v>1.8</v>
       </c>
       <c r="B115">
-        <v>1.87265345563663</v>
+        <v>1.727797061625429</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1271,7 +1271,7 @@
         <v>1.8</v>
       </c>
       <c r="B116">
-        <v>1.852291720246043</v>
+        <v>1.738437649350005</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1279,7 +1279,7 @@
         <v>1.8</v>
       </c>
       <c r="B117">
-        <v>1.914328793251968</v>
+        <v>1.787377855506646</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1287,7 +1287,7 @@
         <v>1.8</v>
       </c>
       <c r="B118">
-        <v>1.894778992313014</v>
+        <v>1.781322514407457</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1295,7 +1295,7 @@
         <v>1.8</v>
       </c>
       <c r="B119">
-        <v>1.897453981570671</v>
+        <v>1.770915057159294</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1303,7 +1303,7 @@
         <v>1.8</v>
       </c>
       <c r="B120">
-        <v>1.792619385148079</v>
+        <v>1.730810955214038</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1311,7 +1311,7 @@
         <v>2.1</v>
       </c>
       <c r="B121">
-        <v>2.079343562681863</v>
+        <v>2.182283497869066</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1319,7 +1319,7 @@
         <v>2.1</v>
       </c>
       <c r="B122">
-        <v>2.125534596483007</v>
+        <v>2.152191100068503</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1327,7 +1327,7 @@
         <v>2.1</v>
       </c>
       <c r="B123">
-        <v>2.092318899380103</v>
+        <v>2.13227915500497</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1335,7 +1335,7 @@
         <v>2.1</v>
       </c>
       <c r="B124">
-        <v>2.147264477514028</v>
+        <v>2.230432567590134</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1343,7 +1343,7 @@
         <v>2.1</v>
       </c>
       <c r="B125">
-        <v>2.182063474259948</v>
+        <v>2.15197018655072</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1351,7 +1351,7 @@
         <v>2.1</v>
       </c>
       <c r="B126">
-        <v>2.05896941413117</v>
+        <v>2.165462314798597</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1359,7 +1359,7 @@
         <v>2.1</v>
       </c>
       <c r="B127">
-        <v>2.194039238870623</v>
+        <v>2.17265001663835</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1367,7 +1367,7 @@
         <v>2.1</v>
       </c>
       <c r="B128">
-        <v>2.161797366524212</v>
+        <v>2.188346629073576</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1375,7 +1375,7 @@
         <v>2.1</v>
       </c>
       <c r="B129">
-        <v>2.137527843613867</v>
+        <v>2.159575778074359</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1383,7 +1383,7 @@
         <v>2.1</v>
       </c>
       <c r="B130">
-        <v>2.134100490631617</v>
+        <v>2.124859566878031</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1391,7 +1391,7 @@
         <v>2.1</v>
       </c>
       <c r="B131">
-        <v>2.205415758612894</v>
+        <v>2.186966669248755</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1399,7 +1399,7 @@
         <v>2.1</v>
       </c>
       <c r="B132">
-        <v>2.173347194564506</v>
+        <v>2.149959399068643</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1407,7 +1407,7 @@
         <v>2.1</v>
       </c>
       <c r="B133">
-        <v>2.240949145110619</v>
+        <v>2.185921201794941</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1415,7 +1415,7 @@
         <v>2.1</v>
       </c>
       <c r="B134">
-        <v>2.321409950512816</v>
+        <v>2.202064364191681</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1423,7 +1423,7 @@
         <v>2.1</v>
       </c>
       <c r="B135">
-        <v>2.208483842050477</v>
+        <v>2.222318504062551</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1431,7 +1431,7 @@
         <v>2.1</v>
       </c>
       <c r="B136">
-        <v>2.226228216320266</v>
+        <v>2.175988065202822</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1439,7 +1439,7 @@
         <v>2.1</v>
       </c>
       <c r="B137">
-        <v>2.336258459387622</v>
+        <v>2.232031483551521</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1447,7 +1447,7 @@
         <v>2.1</v>
       </c>
       <c r="B138">
-        <v>2.205660924427235</v>
+        <v>2.207751521201505</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1455,7 +1455,7 @@
         <v>2.1</v>
       </c>
       <c r="B139">
-        <v>2.2226062981917</v>
+        <v>2.191509980019663</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1463,7 +1463,7 @@
         <v>2.1</v>
       </c>
       <c r="B140">
-        <v>2.263198919741392</v>
+        <v>2.208289652376372</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1471,7 +1471,7 @@
         <v>2.4</v>
       </c>
       <c r="B141">
-        <v>2.290792894282554</v>
+        <v>2.495608069464515</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1479,7 +1479,7 @@
         <v>2.4</v>
       </c>
       <c r="B142">
-        <v>2.37322786851604</v>
+        <v>2.488150265400911</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1487,7 +1487,7 @@
         <v>2.4</v>
       </c>
       <c r="B143">
-        <v>2.245851503064927</v>
+        <v>2.392471600915024</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1495,7 +1495,7 @@
         <v>2.4</v>
       </c>
       <c r="B144">
-        <v>2.225233393228343</v>
+        <v>2.429636866858722</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1503,7 +1503,7 @@
         <v>2.4</v>
       </c>
       <c r="B145">
-        <v>2.324856704978536</v>
+        <v>2.495092136768679</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1511,7 +1511,7 @@
         <v>2.4</v>
       </c>
       <c r="B146">
-        <v>2.260309830849401</v>
+        <v>2.42386965420302</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1519,7 +1519,7 @@
         <v>2.4</v>
       </c>
       <c r="B147">
-        <v>2.294271309059582</v>
+        <v>2.417491244506504</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1527,7 +1527,7 @@
         <v>2.4</v>
       </c>
       <c r="B148">
-        <v>2.338858808955806</v>
+        <v>2.391436882171203</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1535,7 +1535,7 @@
         <v>2.4</v>
       </c>
       <c r="B149">
-        <v>2.277668912964259</v>
+        <v>2.42804225463917</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1543,7 +1543,7 @@
         <v>2.4</v>
       </c>
       <c r="B150">
-        <v>2.395250220975143</v>
+        <v>2.45076711197434</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1551,7 +1551,7 @@
         <v>2.4</v>
       </c>
       <c r="B151">
-        <v>2.373096974472801</v>
+        <v>2.475413101410838</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1559,7 +1559,7 @@
         <v>2.4</v>
       </c>
       <c r="B152">
-        <v>2.321249395384498</v>
+        <v>2.441500259240796</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1567,7 +1567,7 @@
         <v>2.4</v>
       </c>
       <c r="B153">
-        <v>2.323238941224439</v>
+        <v>2.445853077738017</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1575,7 +1575,7 @@
         <v>2.4</v>
       </c>
       <c r="B154">
-        <v>2.413021939990003</v>
+        <v>2.492797531534229</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1583,7 +1583,7 @@
         <v>2.4</v>
       </c>
       <c r="B155">
-        <v>2.373014203182962</v>
+        <v>2.49433976234767</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1591,7 +1591,7 @@
         <v>2.4</v>
       </c>
       <c r="B156">
-        <v>2.386613308136553</v>
+        <v>2.482487506046591</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1599,7 +1599,7 @@
         <v>2.4</v>
       </c>
       <c r="B157">
-        <v>2.28850764482825</v>
+        <v>2.419661526033768</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1607,7 +1607,7 @@
         <v>2.4</v>
       </c>
       <c r="B158">
-        <v>2.337782936955954</v>
+        <v>2.400822951192172</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1615,7 +1615,7 @@
         <v>2.4</v>
       </c>
       <c r="B159">
-        <v>2.371850540196931</v>
+        <v>2.47218434231202</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1623,7 +1623,7 @@
         <v>2.4</v>
       </c>
       <c r="B160">
-        <v>2.313785449975143</v>
+        <v>2.480772258574737</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1631,7 +1631,7 @@
         <v>2.7</v>
       </c>
       <c r="B161">
-        <v>2.951577540563775</v>
+        <v>2.778001288416424</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1639,7 +1639,7 @@
         <v>2.7</v>
       </c>
       <c r="B162">
-        <v>2.876319749243351</v>
+        <v>2.726661632444681</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1647,7 +1647,7 @@
         <v>2.7</v>
       </c>
       <c r="B163">
-        <v>2.870359436605177</v>
+        <v>2.710295035290429</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1655,7 +1655,7 @@
         <v>2.7</v>
       </c>
       <c r="B164">
-        <v>2.949687649928947</v>
+        <v>2.797154427419439</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1663,7 +1663,7 @@
         <v>2.7</v>
       </c>
       <c r="B165">
-        <v>2.899382479849685</v>
+        <v>2.708753704029572</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1671,7 +1671,7 @@
         <v>2.7</v>
       </c>
       <c r="B166">
-        <v>2.862070997905597</v>
+        <v>2.728437083504805</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1679,7 +1679,7 @@
         <v>2.7</v>
       </c>
       <c r="B167">
-        <v>2.906387001345685</v>
+        <v>2.723311947294093</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1687,7 +1687,7 @@
         <v>2.7</v>
       </c>
       <c r="B168">
-        <v>2.956882118111942</v>
+        <v>2.731391576659526</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1695,7 +1695,7 @@
         <v>2.7</v>
       </c>
       <c r="B169">
-        <v>2.851835365890302</v>
+        <v>2.670822934603096</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1703,7 +1703,7 @@
         <v>2.7</v>
       </c>
       <c r="B170">
-        <v>2.789835913356185</v>
+        <v>2.702081440868391</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1711,7 +1711,7 @@
         <v>2.7</v>
       </c>
       <c r="B171">
-        <v>2.676576127584688</v>
+        <v>2.679951566146721</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1719,7 +1719,7 @@
         <v>2.7</v>
       </c>
       <c r="B172">
-        <v>2.687574012688962</v>
+        <v>2.67400840263993</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1727,7 +1727,7 @@
         <v>2.7</v>
       </c>
       <c r="B173">
-        <v>2.746523585244177</v>
+        <v>2.678221813194887</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1735,7 +1735,7 @@
         <v>2.7</v>
       </c>
       <c r="B174">
-        <v>2.671114255899809</v>
+        <v>2.628082034112277</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1743,7 +1743,7 @@
         <v>2.7</v>
       </c>
       <c r="B175">
-        <v>2.729740508855173</v>
+        <v>2.680486826516035</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1751,7 +1751,7 @@
         <v>2.7</v>
       </c>
       <c r="B176">
-        <v>2.724538159968517</v>
+        <v>2.664167902408749</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1759,7 +1759,7 @@
         <v>2.7</v>
       </c>
       <c r="B177">
-        <v>2.741883321357001</v>
+        <v>2.69502791385211</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1767,7 +1767,7 @@
         <v>2.7</v>
       </c>
       <c r="B178">
-        <v>2.7529789438058</v>
+        <v>2.682695602809673</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1775,7 +1775,7 @@
         <v>2.7</v>
       </c>
       <c r="B179">
-        <v>2.736164041117149</v>
+        <v>2.674712066240287</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1783,7 +1783,7 @@
         <v>2.7</v>
       </c>
       <c r="B180">
-        <v>2.717753918306059</v>
+        <v>2.716955622907549</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1791,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="B181">
-        <v>2.947136557570495</v>
+        <v>2.977922405351118</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1799,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="B182">
-        <v>2.997751176470743</v>
+        <v>2.923401334647342</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1807,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="B183">
-        <v>2.989905320451967</v>
+        <v>2.881313443709668</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1815,7 +1815,7 @@
         <v>3</v>
       </c>
       <c r="B184">
-        <v>2.941569732508512</v>
+        <v>2.899620093107433</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1823,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="B185">
-        <v>2.982812375327526</v>
+        <v>2.937723117751033</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1831,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="B186">
-        <v>2.96065862493937</v>
+        <v>2.947178854876001</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1839,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="B187">
-        <v>3.078862418719766</v>
+        <v>2.95079204203531</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1847,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="B188">
-        <v>3.001312697212008</v>
+        <v>2.943613768876728</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1855,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="B189">
-        <v>3.02121565476552</v>
+        <v>2.88723845088404</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1863,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="B190">
-        <v>3.030995173953166</v>
+        <v>2.967215099920299</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1871,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="B191">
-        <v>2.831679041208808</v>
+        <v>2.867042504083889</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>3</v>
       </c>
       <c r="B192">
-        <v>2.881539763809897</v>
+        <v>2.814612233234604</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1887,7 +1887,7 @@
         <v>3</v>
       </c>
       <c r="B193">
-        <v>2.894704125640068</v>
+        <v>2.941680635409718</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1895,7 +1895,7 @@
         <v>3</v>
       </c>
       <c r="B194">
-        <v>2.722477320449009</v>
+        <v>2.809603661813892</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1903,7 +1903,7 @@
         <v>3</v>
       </c>
       <c r="B195">
-        <v>2.901408808267433</v>
+        <v>2.93849017404967</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1911,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="B196">
-        <v>2.646428931655358</v>
+        <v>2.921502586994126</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>3</v>
       </c>
       <c r="B197">
-        <v>2.718425528997848</v>
+        <v>2.918930006743758</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1927,7 +1927,7 @@
         <v>3</v>
       </c>
       <c r="B198">
-        <v>2.762745838513936</v>
+        <v>2.768086852753551</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1935,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B199">
-        <v>2.875037651414381</v>
+        <v>2.781996035121966</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1943,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="B200">
-        <v>2.865382519976045</v>
+        <v>2.885084742305622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hard Press Force Regression
</commit_message>
<xml_diff>
--- a/RegressionResults.xlsx
+++ b/RegressionResults.xlsx
@@ -351,7 +351,7 @@
         <v>0.3</v>
       </c>
       <c r="B1">
-        <v>0.2244049146159082</v>
+        <v>0.3158148626316257</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -359,7 +359,7 @@
         <v>0.3</v>
       </c>
       <c r="B2">
-        <v>0.2966943850757304</v>
+        <v>0.3070743832391252</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -367,7 +367,7 @@
         <v>0.3</v>
       </c>
       <c r="B3">
-        <v>0.2841325605766061</v>
+        <v>0.308086293762039</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -375,7 +375,7 @@
         <v>0.3</v>
       </c>
       <c r="B4">
-        <v>0.2461213919509468</v>
+        <v>0.3092508016746884</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -383,7 +383,7 @@
         <v>0.3</v>
       </c>
       <c r="B5">
-        <v>0.2586599311173301</v>
+        <v>0.3378443432764913</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -391,7 +391,7 @@
         <v>0.3</v>
       </c>
       <c r="B6">
-        <v>0.257391690361052</v>
+        <v>0.3179561294739084</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -399,7 +399,7 @@
         <v>0.3</v>
       </c>
       <c r="B7">
-        <v>0.3259311987765785</v>
+        <v>0.3083164944194161</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -407,7 +407,7 @@
         <v>0.3</v>
       </c>
       <c r="B8">
-        <v>0.2512733543594496</v>
+        <v>0.2741463083924245</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -415,7 +415,7 @@
         <v>0.3</v>
       </c>
       <c r="B9">
-        <v>0.2549879519166294</v>
+        <v>0.3282443403443671</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -423,7 +423,7 @@
         <v>0.3</v>
       </c>
       <c r="B10">
-        <v>0.2504928486289062</v>
+        <v>0.3128567792809445</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -431,7 +431,7 @@
         <v>0.3</v>
       </c>
       <c r="B11">
-        <v>0.2723379812052493</v>
+        <v>0.273735740591337</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -439,7 +439,7 @@
         <v>0.3</v>
       </c>
       <c r="B12">
-        <v>0.2663861495484068</v>
+        <v>0.2597410698232734</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -447,7 +447,7 @@
         <v>0.3</v>
       </c>
       <c r="B13">
-        <v>0.2786552465379439</v>
+        <v>0.2597967770175731</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -455,7 +455,7 @@
         <v>0.3</v>
       </c>
       <c r="B14">
-        <v>0.274846017359172</v>
+        <v>0.2673801321996976</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -463,7 +463,7 @@
         <v>0.3</v>
       </c>
       <c r="B15">
-        <v>0.2960167444859172</v>
+        <v>0.2628074969474843</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -471,7 +471,7 @@
         <v>0.3</v>
       </c>
       <c r="B16">
-        <v>0.2868891749835374</v>
+        <v>0.2567411766905521</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -479,7 +479,7 @@
         <v>0.3</v>
       </c>
       <c r="B17">
-        <v>0.2823203520770745</v>
+        <v>0.2457094143753173</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -487,7 +487,7 @@
         <v>0.3</v>
       </c>
       <c r="B18">
-        <v>0.2860781212899837</v>
+        <v>0.2437002873033514</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -495,7 +495,7 @@
         <v>0.3</v>
       </c>
       <c r="B19">
-        <v>0.2884366226230255</v>
+        <v>0.2561170959632249</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -503,7 +503,7 @@
         <v>0.3</v>
       </c>
       <c r="B20">
-        <v>0.2753854648678993</v>
+        <v>0.2607568907515723</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -511,7 +511,7 @@
         <v>0.6</v>
       </c>
       <c r="B21">
-        <v>0.9567567476243846</v>
+        <v>0.6720516427448597</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -519,7 +519,7 @@
         <v>0.6</v>
       </c>
       <c r="B22">
-        <v>0.9369184755524351</v>
+        <v>0.6720755724782785</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -527,7 +527,7 @@
         <v>0.6</v>
       </c>
       <c r="B23">
-        <v>0.9752133735339363</v>
+        <v>0.6659728011583526</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -535,7 +535,7 @@
         <v>0.6</v>
       </c>
       <c r="B24">
-        <v>0.9476815634142541</v>
+        <v>0.6672970771824132</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -543,7 +543,7 @@
         <v>0.6</v>
       </c>
       <c r="B25">
-        <v>0.9509101927322186</v>
+        <v>0.6953487708750838</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -551,7 +551,7 @@
         <v>0.6</v>
       </c>
       <c r="B26">
-        <v>0.9797065874858975</v>
+        <v>0.670146389251552</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -559,7 +559,7 @@
         <v>0.6</v>
       </c>
       <c r="B27">
-        <v>0.9954497039790526</v>
+        <v>0.6773679430470785</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -567,7 +567,7 @@
         <v>0.6</v>
       </c>
       <c r="B28">
-        <v>0.9827678749595909</v>
+        <v>0.675563462663229</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -575,7 +575,7 @@
         <v>0.6</v>
       </c>
       <c r="B29">
-        <v>0.9525434326041196</v>
+        <v>0.6694553513189074</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -583,7 +583,7 @@
         <v>0.6</v>
       </c>
       <c r="B30">
-        <v>0.9692783345695077</v>
+        <v>0.6702881030675123</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -591,7 +591,7 @@
         <v>0.6</v>
       </c>
       <c r="B31">
-        <v>0.7311670281391756</v>
+        <v>0.6328453014906688</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -599,7 +599,7 @@
         <v>0.6</v>
       </c>
       <c r="B32">
-        <v>0.7214513540791607</v>
+        <v>0.6231388728618916</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -607,7 +607,7 @@
         <v>0.6</v>
       </c>
       <c r="B33">
-        <v>0.7577111274251549</v>
+        <v>0.6382623837872134</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -615,7 +615,7 @@
         <v>0.6</v>
       </c>
       <c r="B34">
-        <v>0.7602944194184227</v>
+        <v>0.6209309443169126</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -623,7 +623,7 @@
         <v>0.6</v>
       </c>
       <c r="B35">
-        <v>0.7497657886383182</v>
+        <v>0.6395117698141666</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -631,7 +631,7 @@
         <v>0.6</v>
       </c>
       <c r="B36">
-        <v>0.7630017045606641</v>
+        <v>0.6512955239507094</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -639,7 +639,7 @@
         <v>0.6</v>
       </c>
       <c r="B37">
-        <v>0.7730196584628746</v>
+        <v>0.6455774469986872</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -647,7 +647,7 @@
         <v>0.6</v>
       </c>
       <c r="B38">
-        <v>0.8292102833790396</v>
+        <v>0.6342123362952492</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -655,7 +655,7 @@
         <v>0.6</v>
       </c>
       <c r="B39">
-        <v>0.741655882791449</v>
+        <v>0.6424000608612681</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -663,7 +663,7 @@
         <v>0.6</v>
       </c>
       <c r="B40">
-        <v>0.8277760975738393</v>
+        <v>0.6369093832723303</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -671,7 +671,7 @@
         <v>0.9</v>
       </c>
       <c r="B41">
-        <v>1.113178433379558</v>
+        <v>0.9438797887102246</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -679,7 +679,7 @@
         <v>0.9</v>
       </c>
       <c r="B42">
-        <v>1.119814876827882</v>
+        <v>0.9397711919335137</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -687,7 +687,7 @@
         <v>0.9</v>
       </c>
       <c r="B43">
-        <v>1.13244169552259</v>
+        <v>0.9531804413906046</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -695,7 +695,7 @@
         <v>0.9</v>
       </c>
       <c r="B44">
-        <v>1.124638494108494</v>
+        <v>0.9551347788152154</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -703,7 +703,7 @@
         <v>0.9</v>
       </c>
       <c r="B45">
-        <v>1.13606758556665</v>
+        <v>0.9411629728125963</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -711,7 +711,7 @@
         <v>0.9</v>
       </c>
       <c r="B46">
-        <v>1.089512586585638</v>
+        <v>0.9316713377829695</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -719,7 +719,7 @@
         <v>0.9</v>
       </c>
       <c r="B47">
-        <v>1.143385092072646</v>
+        <v>0.9384226883392224</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -727,7 +727,7 @@
         <v>0.9</v>
       </c>
       <c r="B48">
-        <v>1.081033258374178</v>
+        <v>0.9429613517518309</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -735,7 +735,7 @@
         <v>0.9</v>
       </c>
       <c r="B49">
-        <v>1.087931894231743</v>
+        <v>0.9373585291860618</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -743,7 +743,7 @@
         <v>0.9</v>
       </c>
       <c r="B50">
-        <v>1.078409143499878</v>
+        <v>0.9366856973743865</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -751,7 +751,7 @@
         <v>0.9</v>
       </c>
       <c r="B51">
-        <v>0.8476493300129482</v>
+        <v>0.9662133280738134</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -759,7 +759,7 @@
         <v>0.9</v>
       </c>
       <c r="B52">
-        <v>0.8809575396146641</v>
+        <v>0.9616022611822062</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -767,7 +767,7 @@
         <v>0.9</v>
       </c>
       <c r="B53">
-        <v>0.8455715455120751</v>
+        <v>0.9574048978182779</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -775,7 +775,7 @@
         <v>0.9</v>
       </c>
       <c r="B54">
-        <v>0.7944703363004484</v>
+        <v>0.9710748464303618</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -783,7 +783,7 @@
         <v>0.9</v>
       </c>
       <c r="B55">
-        <v>0.8390257662130134</v>
+        <v>0.9747243650617599</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -791,7 +791,7 @@
         <v>0.9</v>
       </c>
       <c r="B56">
-        <v>0.8628089257266272</v>
+        <v>0.9591556070530822</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -799,7 +799,7 @@
         <v>0.9</v>
       </c>
       <c r="B57">
-        <v>0.7710910676110356</v>
+        <v>0.9498069773540676</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -807,7 +807,7 @@
         <v>0.9</v>
       </c>
       <c r="B58">
-        <v>0.84213553014138</v>
+        <v>0.9594117853696875</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -815,7 +815,7 @@
         <v>0.9</v>
       </c>
       <c r="B59">
-        <v>0.8465664312561638</v>
+        <v>0.9520656947256998</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -823,7 +823,7 @@
         <v>0.9</v>
       </c>
       <c r="B60">
-        <v>0.8821682804450295</v>
+        <v>0.9876257197679963</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -831,7 +831,7 @@
         <v>1.2</v>
       </c>
       <c r="B61">
-        <v>1.325214853092706</v>
+        <v>1.283927332138705</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -839,7 +839,7 @@
         <v>1.2</v>
       </c>
       <c r="B62">
-        <v>1.229746492657904</v>
+        <v>1.285462731370106</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -847,7 +847,7 @@
         <v>1.2</v>
       </c>
       <c r="B63">
-        <v>1.296492368661867</v>
+        <v>1.306145416467936</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -855,7 +855,7 @@
         <v>1.2</v>
       </c>
       <c r="B64">
-        <v>1.285224397640298</v>
+        <v>1.291266695223646</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -863,7 +863,7 @@
         <v>1.2</v>
       </c>
       <c r="B65">
-        <v>1.29569701553315</v>
+        <v>1.299785944321258</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -871,7 +871,7 @@
         <v>1.2</v>
       </c>
       <c r="B66">
-        <v>1.304457332121114</v>
+        <v>1.269914497475928</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -879,7 +879,7 @@
         <v>1.2</v>
       </c>
       <c r="B67">
-        <v>1.316381043502975</v>
+        <v>1.264003352626237</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -887,7 +887,7 @@
         <v>1.2</v>
       </c>
       <c r="B68">
-        <v>1.261809784173537</v>
+        <v>1.282263196323869</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -895,7 +895,7 @@
         <v>1.2</v>
       </c>
       <c r="B69">
-        <v>1.315708898749855</v>
+        <v>1.29597935530944</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -903,7 +903,7 @@
         <v>1.2</v>
       </c>
       <c r="B70">
-        <v>1.286543615954848</v>
+        <v>1.295348650410338</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -911,7 +911,7 @@
         <v>1.2</v>
       </c>
       <c r="B71">
-        <v>1.396385483695001</v>
+        <v>1.180887909516312</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -919,7 +919,7 @@
         <v>1.2</v>
       </c>
       <c r="B72">
-        <v>1.358687872728843</v>
+        <v>1.183648506476057</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -927,7 +927,7 @@
         <v>1.2</v>
       </c>
       <c r="B73">
-        <v>1.389910198365495</v>
+        <v>1.177246307689471</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -935,7 +935,7 @@
         <v>1.2</v>
       </c>
       <c r="B74">
-        <v>1.395722089557511</v>
+        <v>1.167460632776637</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -943,7 +943,7 @@
         <v>1.2</v>
       </c>
       <c r="B75">
-        <v>1.404384643787551</v>
+        <v>1.147353870782619</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -951,7 +951,7 @@
         <v>1.2</v>
       </c>
       <c r="B76">
-        <v>1.382893017324087</v>
+        <v>1.168866525985515</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -959,7 +959,7 @@
         <v>1.2</v>
       </c>
       <c r="B77">
-        <v>1.387109730679059</v>
+        <v>1.16560455103107</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -967,7 +967,7 @@
         <v>1.2</v>
       </c>
       <c r="B78">
-        <v>1.378225959106202</v>
+        <v>1.168648481447992</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -975,7 +975,7 @@
         <v>1.2</v>
       </c>
       <c r="B79">
-        <v>1.405054707522149</v>
+        <v>1.170083156352999</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -983,7 +983,7 @@
         <v>1.2</v>
       </c>
       <c r="B80">
-        <v>1.382692762728911</v>
+        <v>1.174746192219415</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -991,7 +991,7 @@
         <v>1.5</v>
       </c>
       <c r="B81">
-        <v>1.519949567282465</v>
+        <v>1.664806243253966</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -999,7 +999,7 @@
         <v>1.5</v>
       </c>
       <c r="B82">
-        <v>1.533925907495531</v>
+        <v>1.683586820738566</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1007,7 +1007,7 @@
         <v>1.5</v>
       </c>
       <c r="B83">
-        <v>1.514656491932222</v>
+        <v>1.681807065624995</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1015,7 +1015,7 @@
         <v>1.5</v>
       </c>
       <c r="B84">
-        <v>1.477481983750496</v>
+        <v>1.688463172751192</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1023,7 +1023,7 @@
         <v>1.5</v>
       </c>
       <c r="B85">
-        <v>1.459509504185802</v>
+        <v>1.689274404134356</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1031,7 +1031,7 @@
         <v>1.5</v>
       </c>
       <c r="B86">
-        <v>1.504534449453706</v>
+        <v>1.680541208597784</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1039,7 +1039,7 @@
         <v>1.5</v>
       </c>
       <c r="B87">
-        <v>1.475914230032065</v>
+        <v>1.689133603583572</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1047,7 +1047,7 @@
         <v>1.5</v>
       </c>
       <c r="B88">
-        <v>1.47569973841794</v>
+        <v>1.690800918714859</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1055,7 +1055,7 @@
         <v>1.5</v>
       </c>
       <c r="B89">
-        <v>1.492951699001821</v>
+        <v>1.698770309133228</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1063,7 +1063,7 @@
         <v>1.5</v>
       </c>
       <c r="B90">
-        <v>1.511722385280024</v>
+        <v>1.674123797836201</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1071,7 +1071,7 @@
         <v>1.5</v>
       </c>
       <c r="B91">
-        <v>1.458013303765713</v>
+        <v>1.486017970272043</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1079,7 +1079,7 @@
         <v>1.5</v>
       </c>
       <c r="B92">
-        <v>1.456531483572662</v>
+        <v>1.46615769071866</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1087,7 +1087,7 @@
         <v>1.5</v>
       </c>
       <c r="B93">
-        <v>1.439353102966979</v>
+        <v>1.465034363204356</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1095,7 +1095,7 @@
         <v>1.5</v>
       </c>
       <c r="B94">
-        <v>1.460197791533025</v>
+        <v>1.465705647693798</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1103,7 +1103,7 @@
         <v>1.5</v>
       </c>
       <c r="B95">
-        <v>1.435856058132061</v>
+        <v>1.449488947256801</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1111,7 +1111,7 @@
         <v>1.5</v>
       </c>
       <c r="B96">
-        <v>1.448038975866202</v>
+        <v>1.471055108243076</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1119,7 +1119,7 @@
         <v>1.5</v>
       </c>
       <c r="B97">
-        <v>1.391681384479898</v>
+        <v>1.458367553799803</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1127,7 +1127,7 @@
         <v>1.5</v>
       </c>
       <c r="B98">
-        <v>1.405487161002725</v>
+        <v>1.454765208231616</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1135,7 +1135,7 @@
         <v>1.5</v>
       </c>
       <c r="B99">
-        <v>1.408415131242398</v>
+        <v>1.455867925776068</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1143,7 +1143,7 @@
         <v>1.5</v>
       </c>
       <c r="B100">
-        <v>1.472233491256338</v>
+        <v>1.450499370552702</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1151,7 +1151,7 @@
         <v>1.8</v>
       </c>
       <c r="B101">
-        <v>1.789987751768453</v>
+        <v>1.900424590078695</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1159,7 +1159,7 @@
         <v>1.8</v>
       </c>
       <c r="B102">
-        <v>1.810071783112584</v>
+        <v>1.820494368861403</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1167,7 +1167,7 @@
         <v>1.8</v>
       </c>
       <c r="B103">
-        <v>1.786412341800955</v>
+        <v>1.784454224502839</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1175,7 +1175,7 @@
         <v>1.8</v>
       </c>
       <c r="B104">
-        <v>1.792416123068133</v>
+        <v>1.785650765768365</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1183,7 +1183,7 @@
         <v>1.8</v>
       </c>
       <c r="B105">
-        <v>1.773571900359829</v>
+        <v>1.789171608907515</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1191,7 +1191,7 @@
         <v>1.8</v>
       </c>
       <c r="B106">
-        <v>1.791232965615264</v>
+        <v>1.766333765069373</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1199,7 +1199,7 @@
         <v>1.8</v>
       </c>
       <c r="B107">
-        <v>1.794507787191275</v>
+        <v>1.768589998633736</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1207,7 +1207,7 @@
         <v>1.8</v>
       </c>
       <c r="B108">
-        <v>1.761265770277382</v>
+        <v>1.775659248254853</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1215,7 +1215,7 @@
         <v>1.8</v>
       </c>
       <c r="B109">
-        <v>1.805750551290381</v>
+        <v>1.769997569794053</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1223,7 +1223,7 @@
         <v>1.8</v>
       </c>
       <c r="B110">
-        <v>1.763610986578727</v>
+        <v>1.770595292929827</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1231,7 +1231,7 @@
         <v>1.8</v>
       </c>
       <c r="B111">
-        <v>1.745122541263489</v>
+        <v>1.783300113886753</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1239,7 +1239,7 @@
         <v>1.8</v>
       </c>
       <c r="B112">
-        <v>1.701120187425618</v>
+        <v>1.776162363263533</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1247,7 +1247,7 @@
         <v>1.8</v>
       </c>
       <c r="B113">
-        <v>1.76479639925543</v>
+        <v>1.785709920570403</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1255,7 +1255,7 @@
         <v>1.8</v>
       </c>
       <c r="B114">
-        <v>1.759680772939097</v>
+        <v>1.780519032595662</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1263,7 +1263,7 @@
         <v>1.8</v>
       </c>
       <c r="B115">
-        <v>1.727797061625429</v>
+        <v>1.806282148956279</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1271,7 +1271,7 @@
         <v>1.8</v>
       </c>
       <c r="B116">
-        <v>1.738437649350005</v>
+        <v>1.804883834949764</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1279,7 +1279,7 @@
         <v>1.8</v>
       </c>
       <c r="B117">
-        <v>1.787377855506646</v>
+        <v>1.792057733099959</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1287,7 +1287,7 @@
         <v>1.8</v>
       </c>
       <c r="B118">
-        <v>1.781322514407457</v>
+        <v>1.781797501978347</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1295,7 +1295,7 @@
         <v>1.8</v>
       </c>
       <c r="B119">
-        <v>1.770915057159294</v>
+        <v>1.81517554842866</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1303,7 +1303,7 @@
         <v>1.8</v>
       </c>
       <c r="B120">
-        <v>1.730810955214038</v>
+        <v>1.780999551498639</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1311,7 +1311,7 @@
         <v>2.1</v>
       </c>
       <c r="B121">
-        <v>2.182283497869066</v>
+        <v>2.109146856531106</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1319,7 +1319,7 @@
         <v>2.1</v>
       </c>
       <c r="B122">
-        <v>2.152191100068503</v>
+        <v>2.101733780517825</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1327,7 +1327,7 @@
         <v>2.1</v>
       </c>
       <c r="B123">
-        <v>2.13227915500497</v>
+        <v>2.119413210475325</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1335,7 +1335,7 @@
         <v>2.1</v>
       </c>
       <c r="B124">
-        <v>2.230432567590134</v>
+        <v>2.116257751797293</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1343,7 +1343,7 @@
         <v>2.1</v>
       </c>
       <c r="B125">
-        <v>2.15197018655072</v>
+        <v>2.119265359977632</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1351,7 +1351,7 @@
         <v>2.1</v>
       </c>
       <c r="B126">
-        <v>2.165462314798597</v>
+        <v>2.102431604830456</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1359,7 +1359,7 @@
         <v>2.1</v>
       </c>
       <c r="B127">
-        <v>2.17265001663835</v>
+        <v>2.076393505974213</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1367,7 +1367,7 @@
         <v>2.1</v>
       </c>
       <c r="B128">
-        <v>2.188346629073576</v>
+        <v>2.088603431610281</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1375,7 +1375,7 @@
         <v>2.1</v>
       </c>
       <c r="B129">
-        <v>2.159575778074359</v>
+        <v>2.093372080917852</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1383,7 +1383,7 @@
         <v>2.1</v>
       </c>
       <c r="B130">
-        <v>2.124859566878031</v>
+        <v>2.09387372796893</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1391,7 +1391,7 @@
         <v>2.1</v>
       </c>
       <c r="B131">
-        <v>2.186966669248755</v>
+        <v>1.851621504440738</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1399,7 +1399,7 @@
         <v>2.1</v>
       </c>
       <c r="B132">
-        <v>2.149959399068643</v>
+        <v>1.844283930789725</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1407,7 +1407,7 @@
         <v>2.1</v>
       </c>
       <c r="B133">
-        <v>2.185921201794941</v>
+        <v>1.841551634131793</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1415,7 +1415,7 @@
         <v>2.1</v>
       </c>
       <c r="B134">
-        <v>2.202064364191681</v>
+        <v>1.851571227121631</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1423,7 +1423,7 @@
         <v>2.1</v>
       </c>
       <c r="B135">
-        <v>2.222318504062551</v>
+        <v>1.845116703892702</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1431,7 +1431,7 @@
         <v>2.1</v>
       </c>
       <c r="B136">
-        <v>2.175988065202822</v>
+        <v>1.830409297431348</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1439,7 +1439,7 @@
         <v>2.1</v>
       </c>
       <c r="B137">
-        <v>2.232031483551521</v>
+        <v>1.848862411265954</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1447,7 +1447,7 @@
         <v>2.1</v>
       </c>
       <c r="B138">
-        <v>2.207751521201505</v>
+        <v>1.830412787939837</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1455,7 +1455,7 @@
         <v>2.1</v>
       </c>
       <c r="B139">
-        <v>2.191509980019663</v>
+        <v>1.826753418537465</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1463,7 +1463,7 @@
         <v>2.1</v>
       </c>
       <c r="B140">
-        <v>2.208289652376372</v>
+        <v>1.817903909733377</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1471,7 +1471,7 @@
         <v>2.4</v>
       </c>
       <c r="B141">
-        <v>2.495608069464515</v>
+        <v>2.40704287780376</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1479,7 +1479,7 @@
         <v>2.4</v>
       </c>
       <c r="B142">
-        <v>2.488150265400911</v>
+        <v>2.414243525431747</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1487,7 +1487,7 @@
         <v>2.4</v>
       </c>
       <c r="B143">
-        <v>2.392471600915024</v>
+        <v>2.408615506822272</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1495,7 +1495,7 @@
         <v>2.4</v>
       </c>
       <c r="B144">
-        <v>2.429636866858722</v>
+        <v>2.40237143234503</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1503,7 +1503,7 @@
         <v>2.4</v>
       </c>
       <c r="B145">
-        <v>2.495092136768679</v>
+        <v>2.42205146395138</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1511,7 +1511,7 @@
         <v>2.4</v>
       </c>
       <c r="B146">
-        <v>2.42386965420302</v>
+        <v>2.418027346647127</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1519,7 +1519,7 @@
         <v>2.4</v>
       </c>
       <c r="B147">
-        <v>2.417491244506504</v>
+        <v>2.424105914369413</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1527,7 +1527,7 @@
         <v>2.4</v>
       </c>
       <c r="B148">
-        <v>2.391436882171203</v>
+        <v>2.413337861132717</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1535,7 +1535,7 @@
         <v>2.4</v>
       </c>
       <c r="B149">
-        <v>2.42804225463917</v>
+        <v>2.404023751873</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1543,7 +1543,7 @@
         <v>2.4</v>
       </c>
       <c r="B150">
-        <v>2.45076711197434</v>
+        <v>2.426243124507867</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1551,7 +1551,7 @@
         <v>2.4</v>
       </c>
       <c r="B151">
-        <v>2.475413101410838</v>
+        <v>2.422816223141324</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1559,7 +1559,7 @@
         <v>2.4</v>
       </c>
       <c r="B152">
-        <v>2.441500259240796</v>
+        <v>2.436294065258256</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1567,7 +1567,7 @@
         <v>2.4</v>
       </c>
       <c r="B153">
-        <v>2.445853077738017</v>
+        <v>2.433379221552909</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1575,7 +1575,7 @@
         <v>2.4</v>
       </c>
       <c r="B154">
-        <v>2.492797531534229</v>
+        <v>2.434370960956144</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1583,7 +1583,7 @@
         <v>2.4</v>
       </c>
       <c r="B155">
-        <v>2.49433976234767</v>
+        <v>2.43069038797694</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1591,7 +1591,7 @@
         <v>2.4</v>
       </c>
       <c r="B156">
-        <v>2.482487506046591</v>
+        <v>2.437886264556012</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1599,7 +1599,7 @@
         <v>2.4</v>
       </c>
       <c r="B157">
-        <v>2.419661526033768</v>
+        <v>2.434629497948304</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1607,7 +1607,7 @@
         <v>2.4</v>
       </c>
       <c r="B158">
-        <v>2.400822951192172</v>
+        <v>2.422267217674266</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1615,7 +1615,7 @@
         <v>2.4</v>
       </c>
       <c r="B159">
-        <v>2.47218434231202</v>
+        <v>2.436831496810523</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1623,7 +1623,7 @@
         <v>2.4</v>
       </c>
       <c r="B160">
-        <v>2.480772258574737</v>
+        <v>2.415666824621623</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1631,7 +1631,7 @@
         <v>2.7</v>
       </c>
       <c r="B161">
-        <v>2.778001288416424</v>
+        <v>2.696730182946735</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1639,7 +1639,7 @@
         <v>2.7</v>
       </c>
       <c r="B162">
-        <v>2.726661632444681</v>
+        <v>2.694053131988088</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1647,7 +1647,7 @@
         <v>2.7</v>
       </c>
       <c r="B163">
-        <v>2.710295035290429</v>
+        <v>2.697130132581518</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1655,7 +1655,7 @@
         <v>2.7</v>
       </c>
       <c r="B164">
-        <v>2.797154427419439</v>
+        <v>2.700681916058124</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1663,7 +1663,7 @@
         <v>2.7</v>
       </c>
       <c r="B165">
-        <v>2.708753704029572</v>
+        <v>2.695438464631503</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1671,7 +1671,7 @@
         <v>2.7</v>
       </c>
       <c r="B166">
-        <v>2.728437083504805</v>
+        <v>2.70204345086791</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1679,7 +1679,7 @@
         <v>2.7</v>
       </c>
       <c r="B167">
-        <v>2.723311947294093</v>
+        <v>2.712133269227822</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1687,7 +1687,7 @@
         <v>2.7</v>
       </c>
       <c r="B168">
-        <v>2.731391576659526</v>
+        <v>2.708510995227866</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1695,7 +1695,7 @@
         <v>2.7</v>
       </c>
       <c r="B169">
-        <v>2.670822934603096</v>
+        <v>2.719817667847881</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1703,7 +1703,7 @@
         <v>2.7</v>
       </c>
       <c r="B170">
-        <v>2.702081440868391</v>
+        <v>2.475663812528782</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1711,7 +1711,7 @@
         <v>2.7</v>
       </c>
       <c r="B171">
-        <v>2.679951566146721</v>
+        <v>2.713417816433652</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1719,7 +1719,7 @@
         <v>2.7</v>
       </c>
       <c r="B172">
-        <v>2.67400840263993</v>
+        <v>2.694506582608485</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1727,7 +1727,7 @@
         <v>2.7</v>
       </c>
       <c r="B173">
-        <v>2.678221813194887</v>
+        <v>2.695148069145673</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1735,7 +1735,7 @@
         <v>2.7</v>
       </c>
       <c r="B174">
-        <v>2.628082034112277</v>
+        <v>2.702415345362971</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1743,7 +1743,7 @@
         <v>2.7</v>
       </c>
       <c r="B175">
-        <v>2.680486826516035</v>
+        <v>2.697395571689627</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1751,7 +1751,7 @@
         <v>2.7</v>
       </c>
       <c r="B176">
-        <v>2.664167902408749</v>
+        <v>2.711316615591753</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1759,7 +1759,7 @@
         <v>2.7</v>
       </c>
       <c r="B177">
-        <v>2.69502791385211</v>
+        <v>2.716344154610913</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1767,7 +1767,7 @@
         <v>2.7</v>
       </c>
       <c r="B178">
-        <v>2.682695602809673</v>
+        <v>2.697578477199984</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1775,7 +1775,7 @@
         <v>2.7</v>
       </c>
       <c r="B179">
-        <v>2.674712066240287</v>
+        <v>2.700258900695825</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1783,7 +1783,7 @@
         <v>2.7</v>
       </c>
       <c r="B180">
-        <v>2.716955622907549</v>
+        <v>2.709613532941132</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1791,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="B181">
-        <v>2.977922405351118</v>
+        <v>2.948168845147782</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1799,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="B182">
-        <v>2.923401334647342</v>
+        <v>2.966007381584134</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1807,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="B183">
-        <v>2.881313443709668</v>
+        <v>2.938267591813578</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1815,7 +1815,7 @@
         <v>3</v>
       </c>
       <c r="B184">
-        <v>2.899620093107433</v>
+        <v>2.94359653204377</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1823,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="B185">
-        <v>2.937723117751033</v>
+        <v>2.960550896762559</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1831,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="B186">
-        <v>2.947178854876001</v>
+        <v>2.934525807028664</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1839,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="B187">
-        <v>2.95079204203531</v>
+        <v>2.945366732632355</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1847,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="B188">
-        <v>2.943613768876728</v>
+        <v>2.932135411307993</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1855,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="B189">
-        <v>2.88723845088404</v>
+        <v>2.945718894070461</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1863,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="B190">
-        <v>2.967215099920299</v>
+        <v>2.935672688649594</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1871,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="B191">
-        <v>2.867042504083889</v>
+        <v>2.950682832246032</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>3</v>
       </c>
       <c r="B192">
-        <v>2.814612233234604</v>
+        <v>2.935902369409074</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1887,7 +1887,7 @@
         <v>3</v>
       </c>
       <c r="B193">
-        <v>2.941680635409718</v>
+        <v>2.955466598138361</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1895,7 +1895,7 @@
         <v>3</v>
       </c>
       <c r="B194">
-        <v>2.809603661813892</v>
+        <v>2.960578925853645</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1903,7 +1903,7 @@
         <v>3</v>
       </c>
       <c r="B195">
-        <v>2.93849017404967</v>
+        <v>2.914285026102003</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1911,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="B196">
-        <v>2.921502586994126</v>
+        <v>2.967241675519613</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>3</v>
       </c>
       <c r="B197">
-        <v>2.918930006743758</v>
+        <v>2.965249935967892</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1927,7 +1927,7 @@
         <v>3</v>
       </c>
       <c r="B198">
-        <v>2.768086852753551</v>
+        <v>2.965596358732355</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1935,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B199">
-        <v>2.781996035121966</v>
+        <v>2.9337283195579</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1943,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="B200">
-        <v>2.885084742305622</v>
+        <v>2.943538256318305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All Microphones 2D Regression Figures
Added the regression results for all 3 microphone regression into the plotting scripts.
</commit_message>
<xml_diff>
--- a/RegressionResults.xlsx
+++ b/RegressionResults.xlsx
@@ -351,7 +351,7 @@
         <v>0.3</v>
       </c>
       <c r="B1">
-        <v>0.282900459286203</v>
+        <v>0.3221525621314227</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -359,7 +359,7 @@
         <v>0.3</v>
       </c>
       <c r="B2">
-        <v>0.3613533602995933</v>
+        <v>0.3565853337866756</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -367,7 +367,7 @@
         <v>0.3</v>
       </c>
       <c r="B3">
-        <v>0.304600306504905</v>
+        <v>0.3563886239038161</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -375,7 +375,7 @@
         <v>0.3</v>
       </c>
       <c r="B4">
-        <v>0.334761917733944</v>
+        <v>0.3417879824691092</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -383,7 +383,7 @@
         <v>0.3</v>
       </c>
       <c r="B5">
-        <v>0.3852036203720888</v>
+        <v>0.322123874682994</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -391,7 +391,7 @@
         <v>0.3</v>
       </c>
       <c r="B6">
-        <v>0.3023371801252839</v>
+        <v>0.3470481603735376</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -399,7 +399,7 @@
         <v>0.3</v>
       </c>
       <c r="B7">
-        <v>0.304911418591729</v>
+        <v>0.3291789685952322</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -407,7 +407,7 @@
         <v>0.3</v>
       </c>
       <c r="B8">
-        <v>0.2920201851409445</v>
+        <v>0.3244970052360623</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -415,7 +415,7 @@
         <v>0.3</v>
       </c>
       <c r="B9">
-        <v>0.3264377926124944</v>
+        <v>0.361062687736089</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -423,7 +423,7 @@
         <v>0.3</v>
       </c>
       <c r="B10">
-        <v>0.2956817140183108</v>
+        <v>0.3360790745907805</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -431,7 +431,7 @@
         <v>0.3</v>
       </c>
       <c r="B11">
-        <v>0.1869041516353687</v>
+        <v>0.2764207441896112</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -439,7 +439,7 @@
         <v>0.3</v>
       </c>
       <c r="B12">
-        <v>0.2052449635832994</v>
+        <v>0.2562775886263871</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -447,7 +447,7 @@
         <v>0.3</v>
       </c>
       <c r="B13">
-        <v>0.1987326400374787</v>
+        <v>0.2278811864720018</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -455,7 +455,7 @@
         <v>0.3</v>
       </c>
       <c r="B14">
-        <v>0.1878951225288912</v>
+        <v>0.2426483425989261</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -463,7 +463,7 @@
         <v>0.3</v>
       </c>
       <c r="B15">
-        <v>0.187484187290639</v>
+        <v>0.259742040274797</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -471,7 +471,7 @@
         <v>0.3</v>
       </c>
       <c r="B16">
-        <v>0.1621104516635481</v>
+        <v>0.2595357074201323</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -479,7 +479,7 @@
         <v>0.3</v>
       </c>
       <c r="B17">
-        <v>0.1718133647238405</v>
+        <v>0.2566211129952021</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -487,7 +487,7 @@
         <v>0.3</v>
       </c>
       <c r="B18">
-        <v>0.1903695976716917</v>
+        <v>0.2621080254895061</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -495,7 +495,7 @@
         <v>0.3</v>
       </c>
       <c r="B19">
-        <v>0.1771585528013444</v>
+        <v>0.2376592363490162</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -503,7 +503,7 @@
         <v>0.3</v>
       </c>
       <c r="B20">
-        <v>0.1672745631394346</v>
+        <v>0.2535825960290667</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -511,7 +511,7 @@
         <v>0.6</v>
       </c>
       <c r="B21">
-        <v>0.5685814589285911</v>
+        <v>0.9526312089965019</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -519,7 +519,7 @@
         <v>0.6</v>
       </c>
       <c r="B22">
-        <v>0.5304867554759565</v>
+        <v>0.9552741167901087</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -527,7 +527,7 @@
         <v>0.6</v>
       </c>
       <c r="B23">
-        <v>0.5382880456325143</v>
+        <v>0.9563507432108358</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -535,7 +535,7 @@
         <v>0.6</v>
       </c>
       <c r="B24">
-        <v>0.5530103997881683</v>
+        <v>0.9525877721677578</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -543,7 +543,7 @@
         <v>0.6</v>
       </c>
       <c r="B25">
-        <v>0.5603276123424457</v>
+        <v>0.9408622919791547</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -551,7 +551,7 @@
         <v>0.6</v>
       </c>
       <c r="B26">
-        <v>0.5705702825361669</v>
+        <v>0.9318029581534526</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -559,7 +559,7 @@
         <v>0.6</v>
       </c>
       <c r="B27">
-        <v>0.4909873351122533</v>
+        <v>0.9252220634486341</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -567,7 +567,7 @@
         <v>0.6</v>
       </c>
       <c r="B28">
-        <v>0.5448042891301714</v>
+        <v>0.8882724263741353</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -575,7 +575,7 @@
         <v>0.6</v>
       </c>
       <c r="B29">
-        <v>0.566417633738024</v>
+        <v>0.90775556444076</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -583,7 +583,7 @@
         <v>0.6</v>
       </c>
       <c r="B30">
-        <v>0.5613883267477884</v>
+        <v>0.8850996089972609</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -591,7 +591,7 @@
         <v>0.6</v>
       </c>
       <c r="B31">
-        <v>0.6038853278381582</v>
+        <v>0.6193517289448058</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -599,7 +599,7 @@
         <v>0.6</v>
       </c>
       <c r="B32">
-        <v>0.6228971594524155</v>
+        <v>0.6320294263399837</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -607,7 +607,7 @@
         <v>0.6</v>
       </c>
       <c r="B33">
-        <v>0.6101532926931186</v>
+        <v>0.6392050910676486</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -615,7 +615,7 @@
         <v>0.6</v>
       </c>
       <c r="B34">
-        <v>0.6094959691870068</v>
+        <v>0.6608586562260348</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -623,7 +623,7 @@
         <v>0.6</v>
       </c>
       <c r="B35">
-        <v>0.5996194988159367</v>
+        <v>0.6823551351292394</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -631,7 +631,7 @@
         <v>0.6</v>
       </c>
       <c r="B36">
-        <v>0.5962456983903122</v>
+        <v>0.6779567177150223</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -639,7 +639,7 @@
         <v>0.6</v>
       </c>
       <c r="B37">
-        <v>0.6144274761848096</v>
+        <v>0.7032664995132683</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -647,7 +647,7 @@
         <v>0.6</v>
       </c>
       <c r="B38">
-        <v>0.6141237325304951</v>
+        <v>0.6041437517711106</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -655,7 +655,7 @@
         <v>0.6</v>
       </c>
       <c r="B39">
-        <v>0.61868406569317</v>
+        <v>0.6361076502852496</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -663,7 +663,7 @@
         <v>0.6</v>
       </c>
       <c r="B40">
-        <v>0.5911322168268776</v>
+        <v>0.6209312402552811</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -671,7 +671,7 @@
         <v>0.9</v>
       </c>
       <c r="B41">
-        <v>1.084388202139204</v>
+        <v>1.009977498199504</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -679,7 +679,7 @@
         <v>0.9</v>
       </c>
       <c r="B42">
-        <v>1.066594357455686</v>
+        <v>1.006598082848776</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -687,7 +687,7 @@
         <v>0.9</v>
       </c>
       <c r="B43">
-        <v>1.06795186675204</v>
+        <v>1.02527121089596</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -695,7 +695,7 @@
         <v>0.9</v>
       </c>
       <c r="B44">
-        <v>1.110594532027561</v>
+        <v>1.01717330421286</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -703,7 +703,7 @@
         <v>0.9</v>
       </c>
       <c r="B45">
-        <v>1.131278236560372</v>
+        <v>1.004688381994306</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -711,7 +711,7 @@
         <v>0.9</v>
       </c>
       <c r="B46">
-        <v>1.094846053724762</v>
+        <v>0.9934171082521308</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -719,7 +719,7 @@
         <v>0.9</v>
       </c>
       <c r="B47">
-        <v>1.085144513223601</v>
+        <v>0.9870352375946447</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -727,7 +727,7 @@
         <v>0.9</v>
       </c>
       <c r="B48">
-        <v>1.110835688581813</v>
+        <v>0.9808020896678085</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -735,7 +735,7 @@
         <v>0.9</v>
       </c>
       <c r="B49">
-        <v>1.103018283567904</v>
+        <v>0.9950772277648423</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -743,7 +743,7 @@
         <v>0.9</v>
       </c>
       <c r="B50">
-        <v>1.121751444214862</v>
+        <v>0.9937844804910971</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -751,7 +751,7 @@
         <v>0.9</v>
       </c>
       <c r="B51">
-        <v>0.8484043013060443</v>
+        <v>0.6873731170954991</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -759,7 +759,7 @@
         <v>0.9</v>
       </c>
       <c r="B52">
-        <v>0.8952880601180127</v>
+        <v>0.6919012050319746</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -767,7 +767,7 @@
         <v>0.9</v>
       </c>
       <c r="B53">
-        <v>0.8945756673095071</v>
+        <v>0.6889635587820566</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -775,7 +775,7 @@
         <v>0.9</v>
       </c>
       <c r="B54">
-        <v>0.9236019720174364</v>
+        <v>0.676066732459861</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -783,7 +783,7 @@
         <v>0.9</v>
       </c>
       <c r="B55">
-        <v>0.9008136607178421</v>
+        <v>0.6955644575681952</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -791,7 +791,7 @@
         <v>0.9</v>
       </c>
       <c r="B56">
-        <v>0.89874201319929</v>
+        <v>0.6936321760838569</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -799,7 +799,7 @@
         <v>0.9</v>
       </c>
       <c r="B57">
-        <v>0.8339957518610497</v>
+        <v>0.6520690262127489</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -807,7 +807,7 @@
         <v>0.9</v>
       </c>
       <c r="B58">
-        <v>0.8734082029914914</v>
+        <v>0.6959267731964125</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -815,7 +815,7 @@
         <v>0.9</v>
       </c>
       <c r="B59">
-        <v>0.8707378184097836</v>
+        <v>0.6890141529604685</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -823,7 +823,7 @@
         <v>0.9</v>
       </c>
       <c r="B60">
-        <v>0.8778488649491121</v>
+        <v>0.6656908025580019</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -831,7 +831,7 @@
         <v>1.2</v>
       </c>
       <c r="B61">
-        <v>1.219069169304221</v>
+        <v>1.106094516586115</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -839,7 +839,7 @@
         <v>1.2</v>
       </c>
       <c r="B62">
-        <v>1.212248730095859</v>
+        <v>1.126250366960409</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -847,7 +847,7 @@
         <v>1.2</v>
       </c>
       <c r="B63">
-        <v>1.226536260851776</v>
+        <v>1.160971208737281</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -855,7 +855,7 @@
         <v>1.2</v>
       </c>
       <c r="B64">
-        <v>1.193894756609565</v>
+        <v>1.144780585876514</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -863,7 +863,7 @@
         <v>1.2</v>
       </c>
       <c r="B65">
-        <v>1.210256225595553</v>
+        <v>1.140074550457336</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -871,7 +871,7 @@
         <v>1.2</v>
       </c>
       <c r="B66">
-        <v>1.203873215365329</v>
+        <v>1.133293313771986</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -879,7 +879,7 @@
         <v>1.2</v>
       </c>
       <c r="B67">
-        <v>1.198898765751954</v>
+        <v>1.153531756815759</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -887,7 +887,7 @@
         <v>1.2</v>
       </c>
       <c r="B68">
-        <v>1.194337157336258</v>
+        <v>1.14588540437204</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -895,7 +895,7 @@
         <v>1.2</v>
       </c>
       <c r="B69">
-        <v>1.209972686746225</v>
+        <v>1.149223629248655</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -903,7 +903,7 @@
         <v>1.2</v>
       </c>
       <c r="B70">
-        <v>1.19507703955583</v>
+        <v>1.141620610660793</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -911,7 +911,7 @@
         <v>1.2</v>
       </c>
       <c r="B71">
-        <v>1.084298135870385</v>
+        <v>1.273681114062579</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -919,7 +919,7 @@
         <v>1.2</v>
       </c>
       <c r="B72">
-        <v>1.089103640193323</v>
+        <v>1.20380739083607</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -927,7 +927,7 @@
         <v>1.2</v>
       </c>
       <c r="B73">
-        <v>1.093154762320085</v>
+        <v>1.216367969537118</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -935,7 +935,7 @@
         <v>1.2</v>
       </c>
       <c r="B74">
-        <v>1.122708010000821</v>
+        <v>1.21482076959867</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -943,7 +943,7 @@
         <v>1.2</v>
       </c>
       <c r="B75">
-        <v>1.095431612530609</v>
+        <v>1.219506376350639</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -951,7 +951,7 @@
         <v>1.2</v>
       </c>
       <c r="B76">
-        <v>1.088434680609931</v>
+        <v>1.209379693115886</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -959,7 +959,7 @@
         <v>1.2</v>
       </c>
       <c r="B77">
-        <v>1.063588293166753</v>
+        <v>1.22289218356441</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -967,7 +967,7 @@
         <v>1.2</v>
       </c>
       <c r="B78">
-        <v>1.087926672845313</v>
+        <v>1.23161506522082</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -975,7 +975,7 @@
         <v>1.2</v>
       </c>
       <c r="B79">
-        <v>1.097932171119713</v>
+        <v>1.269953226971801</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -983,7 +983,7 @@
         <v>1.2</v>
       </c>
       <c r="B80">
-        <v>1.087241564771019</v>
+        <v>1.293173785549237</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -991,7 +991,7 @@
         <v>1.5</v>
       </c>
       <c r="B81">
-        <v>1.450790297232506</v>
+        <v>1.422360513156052</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -999,7 +999,7 @@
         <v>1.5</v>
       </c>
       <c r="B82">
-        <v>1.438857647419462</v>
+        <v>1.397203691244006</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1007,7 +1007,7 @@
         <v>1.5</v>
       </c>
       <c r="B83">
-        <v>1.451366269152457</v>
+        <v>1.413373190935906</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1015,7 +1015,7 @@
         <v>1.5</v>
       </c>
       <c r="B84">
-        <v>1.441311665263414</v>
+        <v>1.441737646654341</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1023,7 +1023,7 @@
         <v>1.5</v>
       </c>
       <c r="B85">
-        <v>1.432325084536153</v>
+        <v>1.424465180298234</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1031,7 +1031,7 @@
         <v>1.5</v>
       </c>
       <c r="B86">
-        <v>1.405332941201758</v>
+        <v>1.456970034273749</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1039,7 +1039,7 @@
         <v>1.5</v>
       </c>
       <c r="B87">
-        <v>1.43296010095088</v>
+        <v>1.413315741957303</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1047,7 +1047,7 @@
         <v>1.5</v>
       </c>
       <c r="B88">
-        <v>1.424064852994265</v>
+        <v>1.440056109043836</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1055,7 +1055,7 @@
         <v>1.5</v>
       </c>
       <c r="B89">
-        <v>1.430574157623631</v>
+        <v>1.463874594622718</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1063,7 +1063,7 @@
         <v>1.5</v>
       </c>
       <c r="B90">
-        <v>1.41492077403178</v>
+        <v>1.502862690217485</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1071,7 +1071,7 @@
         <v>1.5</v>
       </c>
       <c r="B91">
-        <v>1.293759012366222</v>
+        <v>1.546876116284524</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1079,7 +1079,7 @@
         <v>1.5</v>
       </c>
       <c r="B92">
-        <v>1.290822930983814</v>
+        <v>1.530085541297409</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1087,7 +1087,7 @@
         <v>1.5</v>
       </c>
       <c r="B93">
-        <v>1.31478978853267</v>
+        <v>1.534923253161377</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1095,7 +1095,7 @@
         <v>1.5</v>
       </c>
       <c r="B94">
-        <v>1.37303457274421</v>
+        <v>1.520545646326411</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1103,7 +1103,7 @@
         <v>1.5</v>
       </c>
       <c r="B95">
-        <v>1.369019313781535</v>
+        <v>1.489052189075345</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1111,7 +1111,7 @@
         <v>1.5</v>
       </c>
       <c r="B96">
-        <v>1.369429935349185</v>
+        <v>1.500376779139064</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1119,7 +1119,7 @@
         <v>1.5</v>
       </c>
       <c r="B97">
-        <v>1.403956882854282</v>
+        <v>1.481062267213966</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1127,7 +1127,7 @@
         <v>1.5</v>
       </c>
       <c r="B98">
-        <v>1.433372660942648</v>
+        <v>1.485737556344084</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1135,7 +1135,7 @@
         <v>1.5</v>
       </c>
       <c r="B99">
-        <v>1.404220759750985</v>
+        <v>1.47069029870454</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1143,7 +1143,7 @@
         <v>1.5</v>
       </c>
       <c r="B100">
-        <v>1.407577261194827</v>
+        <v>1.467454233331346</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1151,7 +1151,7 @@
         <v>1.8</v>
       </c>
       <c r="B101">
-        <v>1.848757531776558</v>
+        <v>1.839163766177479</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1159,7 +1159,7 @@
         <v>1.8</v>
       </c>
       <c r="B102">
-        <v>1.891102423068049</v>
+        <v>1.827883477254103</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1167,7 +1167,7 @@
         <v>1.8</v>
       </c>
       <c r="B103">
-        <v>1.890873858609489</v>
+        <v>1.836112442038315</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1175,7 +1175,7 @@
         <v>1.8</v>
       </c>
       <c r="B104">
-        <v>1.903485939323779</v>
+        <v>1.824579887208102</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1183,7 +1183,7 @@
         <v>1.8</v>
       </c>
       <c r="B105">
-        <v>1.865628748077008</v>
+        <v>1.822603748047066</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1191,7 +1191,7 @@
         <v>1.8</v>
       </c>
       <c r="B106">
-        <v>1.832828716771346</v>
+        <v>1.83461212116114</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1199,7 +1199,7 @@
         <v>1.8</v>
       </c>
       <c r="B107">
-        <v>1.860728682093987</v>
+        <v>1.816928789597862</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1207,7 +1207,7 @@
         <v>1.8</v>
       </c>
       <c r="B108">
-        <v>1.840934028988708</v>
+        <v>1.838603389074446</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1215,7 +1215,7 @@
         <v>1.8</v>
       </c>
       <c r="B109">
-        <v>1.867530901945239</v>
+        <v>1.843349270422316</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1223,7 +1223,7 @@
         <v>1.8</v>
       </c>
       <c r="B110">
-        <v>1.824929273194021</v>
+        <v>1.850421459230075</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1231,7 +1231,7 @@
         <v>1.8</v>
       </c>
       <c r="B111">
-        <v>1.990260811992333</v>
+        <v>1.730638312001862</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1239,7 +1239,7 @@
         <v>1.8</v>
       </c>
       <c r="B112">
-        <v>1.941290210325378</v>
+        <v>1.745203271682433</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1247,7 +1247,7 @@
         <v>1.8</v>
       </c>
       <c r="B113">
-        <v>1.966095074967423</v>
+        <v>1.733691196478598</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1255,7 +1255,7 @@
         <v>1.8</v>
       </c>
       <c r="B114">
-        <v>2.02450262662541</v>
+        <v>1.718763499988326</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1263,7 +1263,7 @@
         <v>1.8</v>
       </c>
       <c r="B115">
-        <v>1.981987709908327</v>
+        <v>1.723642235699824</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1271,7 +1271,7 @@
         <v>1.8</v>
       </c>
       <c r="B116">
-        <v>1.929593638302988</v>
+        <v>1.694382919680312</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1279,7 +1279,7 @@
         <v>1.8</v>
       </c>
       <c r="B117">
-        <v>1.95231322343083</v>
+        <v>1.710066970441154</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1287,7 +1287,7 @@
         <v>1.8</v>
       </c>
       <c r="B118">
-        <v>1.986744817852992</v>
+        <v>1.694690588857672</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1295,7 +1295,7 @@
         <v>1.8</v>
       </c>
       <c r="B119">
-        <v>2.001143270080643</v>
+        <v>1.702832873410594</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1303,7 +1303,7 @@
         <v>1.8</v>
       </c>
       <c r="B120">
-        <v>2.05237739419038</v>
+        <v>1.678940711046109</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1311,7 +1311,7 @@
         <v>2.1</v>
       </c>
       <c r="B121">
-        <v>2.135407173279368</v>
+        <v>2.133019352545607</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1319,7 +1319,7 @@
         <v>2.1</v>
       </c>
       <c r="B122">
-        <v>2.097284796967558</v>
+        <v>2.117856988190054</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1327,7 +1327,7 @@
         <v>2.1</v>
       </c>
       <c r="B123">
-        <v>2.158638030067282</v>
+        <v>2.13457878377281</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1335,7 +1335,7 @@
         <v>2.1</v>
       </c>
       <c r="B124">
-        <v>2.121343037938443</v>
+        <v>2.12345258553313</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1343,7 +1343,7 @@
         <v>2.1</v>
       </c>
       <c r="B125">
-        <v>2.150289439354333</v>
+        <v>2.142271610697613</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1351,7 +1351,7 @@
         <v>2.1</v>
       </c>
       <c r="B126">
-        <v>2.153905945701286</v>
+        <v>2.130995396680484</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1359,7 +1359,7 @@
         <v>2.1</v>
       </c>
       <c r="B127">
-        <v>2.105733613142944</v>
+        <v>2.160222655976721</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1367,7 +1367,7 @@
         <v>2.1</v>
       </c>
       <c r="B128">
-        <v>2.034111306271711</v>
+        <v>2.172457601032939</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1375,7 +1375,7 @@
         <v>2.1</v>
       </c>
       <c r="B129">
-        <v>2.137888660143056</v>
+        <v>2.166531483840922</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1383,7 +1383,7 @@
         <v>2.1</v>
       </c>
       <c r="B130">
-        <v>2.153531568871998</v>
+        <v>2.090441077348196</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1391,7 +1391,7 @@
         <v>2.1</v>
       </c>
       <c r="B131">
-        <v>2.17859756922825</v>
+        <v>2.093756808891984</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1399,7 +1399,7 @@
         <v>2.1</v>
       </c>
       <c r="B132">
-        <v>2.304070880743212</v>
+        <v>2.059278443117979</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1407,7 +1407,7 @@
         <v>2.1</v>
       </c>
       <c r="B133">
-        <v>2.325487779425635</v>
+        <v>2.086485212455488</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1415,7 +1415,7 @@
         <v>2.1</v>
       </c>
       <c r="B134">
-        <v>2.273868409557095</v>
+        <v>2.09397448826721</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1423,7 +1423,7 @@
         <v>2.1</v>
       </c>
       <c r="B135">
-        <v>2.405700234419386</v>
+        <v>2.094377085698585</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1431,7 +1431,7 @@
         <v>2.1</v>
       </c>
       <c r="B136">
-        <v>2.385732564686455</v>
+        <v>2.086629111958136</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1439,7 +1439,7 @@
         <v>2.1</v>
       </c>
       <c r="B137">
-        <v>2.233186994102021</v>
+        <v>2.083930323157229</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1447,7 +1447,7 @@
         <v>2.1</v>
       </c>
       <c r="B138">
-        <v>2.36096898059915</v>
+        <v>2.077933347856652</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1455,7 +1455,7 @@
         <v>2.1</v>
       </c>
       <c r="B139">
-        <v>2.132073932818006</v>
+        <v>2.074580851077541</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1463,7 +1463,7 @@
         <v>2.1</v>
       </c>
       <c r="B140">
-        <v>2.17702118602577</v>
+        <v>2.07037956310567</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1471,7 +1471,7 @@
         <v>2.4</v>
       </c>
       <c r="B141">
-        <v>2.394125101908842</v>
+        <v>2.32033977168288</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1479,7 +1479,7 @@
         <v>2.4</v>
       </c>
       <c r="B142">
-        <v>2.422108750650714</v>
+        <v>2.320092600207752</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1487,7 +1487,7 @@
         <v>2.4</v>
       </c>
       <c r="B143">
-        <v>2.396062583210028</v>
+        <v>2.30859974163687</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1495,7 +1495,7 @@
         <v>2.4</v>
       </c>
       <c r="B144">
-        <v>2.403417593136148</v>
+        <v>2.308380689514151</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1503,7 +1503,7 @@
         <v>2.4</v>
       </c>
       <c r="B145">
-        <v>2.375313016398927</v>
+        <v>2.325055699444418</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1511,7 +1511,7 @@
         <v>2.4</v>
       </c>
       <c r="B146">
-        <v>2.428345773683897</v>
+        <v>2.315545465338191</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1519,7 +1519,7 @@
         <v>2.4</v>
       </c>
       <c r="B147">
-        <v>2.454488917201078</v>
+        <v>2.310942239895988</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1527,7 +1527,7 @@
         <v>2.4</v>
       </c>
       <c r="B148">
-        <v>2.419676598221235</v>
+        <v>2.302926331186057</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1535,7 +1535,7 @@
         <v>2.4</v>
       </c>
       <c r="B149">
-        <v>2.409083229019747</v>
+        <v>2.33418494888766</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1543,7 +1543,7 @@
         <v>2.4</v>
       </c>
       <c r="B150">
-        <v>2.436284805564654</v>
+        <v>2.330208074405718</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1551,7 +1551,7 @@
         <v>2.4</v>
       </c>
       <c r="B151">
-        <v>2.559872353617545</v>
+        <v>2.392143753744123</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1559,7 +1559,7 @@
         <v>2.4</v>
       </c>
       <c r="B152">
-        <v>2.467588523602175</v>
+        <v>2.447136710693677</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1567,7 +1567,7 @@
         <v>2.4</v>
       </c>
       <c r="B153">
-        <v>2.506012404557957</v>
+        <v>2.422794883861958</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1575,7 +1575,7 @@
         <v>2.4</v>
       </c>
       <c r="B154">
-        <v>2.4941267908586</v>
+        <v>2.440201829274209</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1583,7 +1583,7 @@
         <v>2.4</v>
       </c>
       <c r="B155">
-        <v>2.495349835748407</v>
+        <v>2.420813545714143</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1591,7 +1591,7 @@
         <v>2.4</v>
       </c>
       <c r="B156">
-        <v>2.469262247400676</v>
+        <v>2.444443916338434</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1599,7 +1599,7 @@
         <v>2.4</v>
       </c>
       <c r="B157">
-        <v>2.463577348642593</v>
+        <v>2.441590439029545</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1607,7 +1607,7 @@
         <v>2.4</v>
       </c>
       <c r="B158">
-        <v>2.535484522515589</v>
+        <v>2.42867474664412</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1615,7 +1615,7 @@
         <v>2.4</v>
       </c>
       <c r="B159">
-        <v>2.504438325255785</v>
+        <v>2.457930742802102</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1623,7 +1623,7 @@
         <v>2.4</v>
       </c>
       <c r="B160">
-        <v>2.505566608692621</v>
+        <v>2.439103892840854</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1631,7 +1631,7 @@
         <v>2.7</v>
       </c>
       <c r="B161">
-        <v>2.506604306360453</v>
+        <v>2.717983443750168</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1639,7 +1639,7 @@
         <v>2.7</v>
       </c>
       <c r="B162">
-        <v>2.477324648514383</v>
+        <v>2.722244401337055</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1647,7 +1647,7 @@
         <v>2.7</v>
       </c>
       <c r="B163">
-        <v>2.509065415494931</v>
+        <v>2.694109182923908</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1655,7 +1655,7 @@
         <v>2.7</v>
       </c>
       <c r="B164">
-        <v>2.514955879527654</v>
+        <v>2.679524886464203</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1663,7 +1663,7 @@
         <v>2.7</v>
       </c>
       <c r="B165">
-        <v>2.473628885373861</v>
+        <v>2.683504060020166</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1671,7 +1671,7 @@
         <v>2.7</v>
       </c>
       <c r="B166">
-        <v>2.48272960253631</v>
+        <v>2.718625888109421</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1679,7 +1679,7 @@
         <v>2.7</v>
       </c>
       <c r="B167">
-        <v>2.537758258248618</v>
+        <v>2.692766814772007</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1687,7 +1687,7 @@
         <v>2.7</v>
       </c>
       <c r="B168">
-        <v>2.510670436640473</v>
+        <v>2.734437849170743</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1695,7 +1695,7 @@
         <v>2.7</v>
       </c>
       <c r="B169">
-        <v>2.516818713145239</v>
+        <v>2.647398631775594</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1703,7 +1703,7 @@
         <v>2.7</v>
       </c>
       <c r="B170">
-        <v>2.521043750296027</v>
+        <v>2.680399665223004</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1711,7 +1711,7 @@
         <v>2.7</v>
       </c>
       <c r="B171">
-        <v>2.469829999328251</v>
+        <v>2.652128567368311</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1719,7 +1719,7 @@
         <v>2.7</v>
       </c>
       <c r="B172">
-        <v>2.490259832841812</v>
+        <v>2.652859270864559</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1727,7 +1727,7 @@
         <v>2.7</v>
       </c>
       <c r="B173">
-        <v>2.459956444458124</v>
+        <v>2.666218362305413</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1735,7 +1735,7 @@
         <v>2.7</v>
       </c>
       <c r="B174">
-        <v>2.437385602862665</v>
+        <v>2.661215736294995</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1743,7 +1743,7 @@
         <v>2.7</v>
       </c>
       <c r="B175">
-        <v>2.44169360520796</v>
+        <v>2.66681440947357</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1751,7 +1751,7 @@
         <v>2.7</v>
       </c>
       <c r="B176">
-        <v>2.437667156988725</v>
+        <v>2.656717149201755</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1759,7 +1759,7 @@
         <v>2.7</v>
       </c>
       <c r="B177">
-        <v>2.410989250060009</v>
+        <v>2.688692742261293</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1767,7 +1767,7 @@
         <v>2.7</v>
       </c>
       <c r="B178">
-        <v>2.453463922471236</v>
+        <v>2.630439535217428</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1775,7 +1775,7 @@
         <v>2.7</v>
       </c>
       <c r="B179">
-        <v>2.41651302440764</v>
+        <v>2.67151061090433</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1783,7 +1783,7 @@
         <v>2.7</v>
       </c>
       <c r="B180">
-        <v>2.417014544481973</v>
+        <v>2.684292551811798</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1791,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="B181">
-        <v>3.071372328527771</v>
+        <v>3.001343624995789</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1799,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="B182">
-        <v>3.116933645713971</v>
+        <v>2.98865397432036</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1807,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="B183">
-        <v>3.118513600136628</v>
+        <v>2.994994339857943</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1815,7 +1815,7 @@
         <v>3</v>
       </c>
       <c r="B184">
-        <v>3.134603034311644</v>
+        <v>2.98951920869539</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1823,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="B185">
-        <v>3.143522137490112</v>
+        <v>2.994741139289899</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1831,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="B186">
-        <v>3.142198483867254</v>
+        <v>2.996448700671917</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1839,7 +1839,7 @@
         <v>3</v>
       </c>
       <c r="B187">
-        <v>3.142955085444405</v>
+        <v>2.999698515204032</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1847,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="B188">
-        <v>3.103608568663641</v>
+        <v>2.976447021159415</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1855,7 +1855,7 @@
         <v>3</v>
       </c>
       <c r="B189">
-        <v>3.101181171597572</v>
+        <v>2.985114887258004</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1863,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="B190">
-        <v>3.1482159636114</v>
+        <v>3.01305494679663</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1871,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="B191">
-        <v>2.941256947863538</v>
+        <v>2.872261006539934</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>3</v>
       </c>
       <c r="B192">
-        <v>3.00059972725005</v>
+        <v>2.892187789759732</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1887,7 +1887,7 @@
         <v>3</v>
       </c>
       <c r="B193">
-        <v>2.931646154610018</v>
+        <v>2.885130852937876</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1895,7 +1895,7 @@
         <v>3</v>
       </c>
       <c r="B194">
-        <v>2.927825851635647</v>
+        <v>2.873217178560033</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1903,7 +1903,7 @@
         <v>3</v>
       </c>
       <c r="B195">
-        <v>2.999015807059162</v>
+        <v>2.894870562869402</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1911,7 +1911,7 @@
         <v>3</v>
       </c>
       <c r="B196">
-        <v>2.974465295620734</v>
+        <v>2.942976139059509</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>3</v>
       </c>
       <c r="B197">
-        <v>2.999872319712264</v>
+        <v>2.941975183265099</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1927,7 +1927,7 @@
         <v>3</v>
       </c>
       <c r="B198">
-        <v>2.858461010560696</v>
+        <v>2.910942408106065</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1935,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B199">
-        <v>2.917716723415863</v>
+        <v>2.930401518466292</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1943,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="B200">
-        <v>2.924138157948345</v>
+        <v>2.933306373512397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>